<commit_message>
End of Day Commit COmpleted Lecture 118
</commit_message>
<xml_diff>
--- a/Proposal&Prep/Proposal/Timeline-CompCare.xlsx
+++ b/Proposal&Prep/Proposal/Timeline-CompCare.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liqueseous/ownCloud/Documents/Spring2018/Gui2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liqueseous/ownCloud/Documents/Repos/CompCare/Proposal&amp;Prep/Proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="440" windowWidth="16800" windowHeight="19520" activeTab="1" xr2:uid="{33CF5473-85BB-3144-A4A8-3B09D26BB11C}"/>
+    <workbookView xWindow="10340" yWindow="440" windowWidth="23260" windowHeight="19520" xr2:uid="{33CF5473-85BB-3144-A4A8-3B09D26BB11C}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -57,15 +57,6 @@
     <t>Prototyping - Application Logic Theory</t>
   </si>
   <si>
-    <t>Front End Search - Seek out best possible avenues for implementing the front end portion.</t>
-  </si>
-  <si>
-    <t>Back End Search - Seek out best possible avenues for implementing front end portion.</t>
-  </si>
-  <si>
-    <t>Start Web Interface / Start Back end and Database</t>
-  </si>
-  <si>
     <t>Finish Web Interface / Finish Back end and Database</t>
   </si>
   <si>
@@ -81,14 +72,6 @@
     <t>Prepare Final Submission</t>
   </si>
   <si>
-    <t xml:space="preserve">Delegate Front end and Back end duties Start working on Front and Back end </t>
-  </si>
-  <si>
-    <t>Chris (Front End) 
-Salem (Front End)
-Ryan (Back End)</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -177,6 +160,20 @@
   </si>
   <si>
     <t>Salem</t>
+  </si>
+  <si>
+    <t>Back End Search - Seek out best possible avenues for implementing the back end portion. 
+Start Database setup and backend implementation</t>
+  </si>
+  <si>
+    <t>Front End Search - Seek out best possible avenues for implementing front end portion. 
+Start front end development and server setup</t>
+  </si>
+  <si>
+    <t>Work on backend API and front end features</t>
+  </si>
+  <si>
+    <t>Work on  Web Interface / Backend connections</t>
   </si>
 </sst>
 </file>
@@ -270,7 +267,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -302,126 +299,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
@@ -441,7 +318,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1A5456DD-2F3F-1A48-BC65-C07C480EE32B}" name="Table2" displayName="Table2" ref="A1:E14" totalsRowShown="0">
   <autoFilter ref="A1:E14" xr:uid="{58EFF47E-8FD6-8A46-9AC7-FAEC63966B25}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1A46B701-F463-1349-BCB1-CAB37C549FDC}" name="Week" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{1A46B701-F463-1349-BCB1-CAB37C549FDC}" name="Week" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{9C9BFB96-27EC-1F46-8789-1A5FF7507136}" name="Date"/>
     <tableColumn id="3" xr3:uid="{DCC3D78D-D336-0B4F-8CF3-BE7E79771724}" name="Task"/>
     <tableColumn id="4" xr3:uid="{C026C7D8-0C19-FC46-BFD5-87FE696B4AED}" name="Team Assignment"/>
@@ -657,9 +534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFEA16F-85A0-5C43-AAA0-9B322B3C1F81}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -698,7 +575,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E2" s="5">
         <v>43143</v>
@@ -715,7 +592,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5">
         <v>43150</v>
@@ -732,41 +609,41 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E4" s="5">
         <v>43157</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>43157</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
+      <c r="C5" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5">
         <v>43161</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>43164</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
+      <c r="C6" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6" s="5">
         <v>43168</v>
@@ -780,16 +657,16 @@
         <v>43171</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E7" s="5">
         <v>43175</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -797,16 +674,16 @@
         <v>43178</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5">
         <v>43182</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -814,10 +691,10 @@
         <v>43185</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5">
         <v>43189</v>
@@ -831,10 +708,10 @@
         <v>43192</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E10" s="5">
         <v>43196</v>
@@ -848,10 +725,10 @@
         <v>43199</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E11" s="5">
         <v>43203</v>
@@ -865,10 +742,10 @@
         <v>43206</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E12" s="5">
         <v>43210</v>
@@ -882,10 +759,10 @@
         <v>43213</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E13" s="5">
         <v>43224</v>
@@ -907,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D50B9AA-75D1-234A-B4D3-0BC79E079756}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
@@ -924,19 +801,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -944,7 +821,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>43132</v>
@@ -953,226 +830,226 @@
         <v>43144</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
         <v>43139</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Started">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Started">
       <formula>NOT(ISERROR(SEARCH("Started",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>